<commit_message>
update server option 10
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ID</t>
   </si>
@@ -28,18 +28,6 @@
   </si>
   <si>
     <t>Price</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>prt</t>
-  </si>
-  <si>
-    <t>des</t>
-  </si>
-  <si>
-    <t>123.00</t>
   </si>
 </sst>
 </file>
@@ -406,7 +394,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -434,20 +422,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>